<commit_message>
asynchronous federated search prototype (#13)
global search is implemented as asynchronous federated search and runs on development server
</commit_message>
<xml_diff>
--- a/django/bql/fixtures/skosmosinstances.xlsx
+++ b/django/bql/fixtures/skosmosinstances.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>timeout</t>
+  </si>
+  <si>
+    <t>server down 03.07.2019</t>
+  </si>
+  <si>
+    <t>too slow</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +435,7 @@
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -451,7 +457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -462,7 +468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -473,7 +479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -484,7 +490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -495,7 +501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -506,7 +512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -514,10 +520,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -528,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -537,6 +546,9 @@
       </c>
       <c r="C10" s="2">
         <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>